<commit_message>
Added digikey links to BOM
</commit_message>
<xml_diff>
--- a/sdc-precharge/Project Outputs for sdc_prech_proj/sdc_BOM.xlsx
+++ b/sdc-precharge/Project Outputs for sdc_prech_proj/sdc_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\sfu_phantom\hardware\sdc-precharge\Project Outputs for sdc_prech_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70ABF686-25CD-4DA4-A60A-39B69DFCCA61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201991E9-5B1C-459A-8A72-40118D57223C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0FBBAF34-DDE2-4050-B595-4061748AD0E1}"/>
   </bookViews>
@@ -225,7 +225,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,14 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -278,18 +286,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2594D5E4-8366-4D48-8ADD-0438DDB9BF00}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -614,7 +625,7 @@
     <col min="2" max="2" width="62.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -651,7 +662,7 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="3">
@@ -671,7 +682,7 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3">
@@ -691,7 +702,7 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="3">
@@ -711,7 +722,7 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="3">
@@ -731,7 +742,7 @@
       <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="3">
@@ -751,7 +762,7 @@
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="3">
@@ -771,7 +782,7 @@
       <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="3">
@@ -791,7 +802,7 @@
       <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F9" s="3">
@@ -811,7 +822,7 @@
       <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="3">
@@ -831,7 +842,7 @@
       <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="3">
@@ -851,7 +862,7 @@
       <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F12" s="3">
@@ -871,7 +882,7 @@
       <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F13" s="3">
@@ -891,7 +902,7 @@
       <c r="D14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="3">
@@ -899,7 +910,22 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{E97179DC-64A8-4DD5-9D53-2C523CBE0F65}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{42B55E5C-9392-40AB-BF01-BE9B85631447}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{9E340709-D990-4BC7-892B-49C2CE497C5F}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{81819784-0D06-4A25-8785-9D800AA94E73}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{0982FDFB-682B-4AF5-A0C0-40B96ABA91A4}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{2A2A622C-62C3-4DB2-B0D1-E4A1E8E3C0F9}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{3D14FF51-3AC3-4B8B-B622-BD096F1D936A}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{02E63C77-37C2-4E4F-BA25-CA333CDC1E58}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00C38F57-6AA5-4074-B0A7-F18477D14267}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{347E2A53-6FF8-415E-9057-81EF9221349F}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{5F150B77-E76E-49C9-9C54-558885119151}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{B3A011EA-2D33-4E88-B35E-6EB565F3130E}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{FB774B85-1731-4B75-95F8-AF83A0C25165}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>